<commit_message>
calender and CalendarTest Updated
</commit_message>
<xml_diff>
--- a/src/main/java/com/amazon/TestData/Data.xlsx
+++ b/src/main/java/com/amazon/TestData/Data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr/>
-  <mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHITTI\eclipse-workspace\FreeCRM\src\main\java\com\amazon\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHITTI\git\repository\FreeCRM\src\main\java\com\amazon\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E5EE4-3FEE-4C62-A5D3-19E3C974910F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71F8119-3C7D-4F8A-B550-321961B8D0FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="NewEventInformation" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="2" r:id="rId2"/>
+    <sheet name="HoverOverValues" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -50,13 +51,33 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>New Event</t>
+  </si>
+  <si>
+    <t>View Today</t>
+  </si>
+  <si>
+    <t>Week View</t>
+  </si>
+  <si>
+    <t>Month View</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +105,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,11 +143,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -402,17 +430,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5859375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,12 +488,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCACD60-A5B5-4053-AF26-0D10C976E63A}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14115DD5-DBD5-4D6F-9BF4-C14C59899DBE}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>